<commit_message>
Run experiments and edit plots
</commit_message>
<xml_diff>
--- a/docs/plots.xlsx
+++ b/docs/plots.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user01\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user01\Dropbox\ml_project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="0" windowWidth="18070" windowHeight="7540"/>
+    <workbookView xWindow="3390" yWindow="0" windowWidth="18070" windowHeight="7540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +54,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,8 +62,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,12 +80,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -95,13 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -123,6 +123,458 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>MNIST Full Dataset</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> (RBF)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM-KNN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5555555555555552E-2"/>
+                  <c:y val="5.5555555555555552E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-7E9C-434D-83FC-2BEB41FA81C9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.96909999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97140000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96909999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96730000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95950000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94689999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E9C-434D-83FC-2BEB41FA81C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="377920928"/>
+        <c:axId val="377923224"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="377920928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="377923224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="377923224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="377920928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -531,11 +983,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="497925216"/>
-        <c:axId val="497936368"/>
+        <c:axId val="195009920"/>
+        <c:axId val="195012096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="497925216"/>
+        <c:axId val="195009920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,7 +1027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497936368"/>
+        <c:crossAx val="195012096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -583,7 +1035,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497936368"/>
+        <c:axId val="195012096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -633,463 +1085,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497925216"/>
+        <c:crossAx val="195009920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:rPr>
-              <a:t>MNIST 7291 Dataset</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SVM-KNN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-6.0927329658067714E-2"/>
-                  <c:y val="-4.9907579878921422E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-D5EB-49C4-9BA8-4EC5A98A915C}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>150</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$3:$F$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.94279999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.94820000000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.95269999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.0000">
-                  <c:v>0.96</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.96460000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.9667</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.96679999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.96519999999999995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-92DB-471E-914B-4DF69BA4F3F3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="497959984"/>
-        <c:axId val="497951456"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="497959984"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="497951456"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="497951456"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="497959984"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5.000000000000001E-3"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1205,6 +1203,460 @@
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
+              <a:t>MNIST 7291 Dataset</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM-KNN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.0927329658067714E-2"/>
+                  <c:y val="-4.9907579878921422E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-D5EB-49C4-9BA8-4EC5A98A915C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.94279999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94820000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95269999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.0000">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96460000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96679999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96519999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-92DB-471E-914B-4DF69BA4F3F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="194733184"/>
+        <c:axId val="194734720"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="194733184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="194734720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="194734720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="194733184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5.000000000000001E-3"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t>MNIST</a:t>
             </a:r>
             <a:r>
@@ -1562,11 +2014,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="497945880"/>
-        <c:axId val="497946208"/>
+        <c:axId val="194786432"/>
+        <c:axId val="194788352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="497945880"/>
+        <c:axId val="194786432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,7 +2058,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497946208"/>
+        <c:crossAx val="194788352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1614,7 +2066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497946208"/>
+        <c:axId val="194788352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1664,7 +2116,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497945880"/>
+        <c:crossAx val="194786432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1742,10 +2194,13 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1852,6 +2307,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3361,8 +3853,541 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>298822</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>17929</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7469</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>14940</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -3387,36 +4412,6 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>103728</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>24709</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>417493</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>39651</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="15" name="Chart 14"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
@@ -3425,20 +4420,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>189351</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>54801</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>17238</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>476469</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>75857</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>32181</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvPr id="15" name="Chart 14"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3456,15 +4451,45 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>293075</xdr:colOff>
+      <xdr:colOff>301410</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>166860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>588528</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>1152</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>240781</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>68375</xdr:rowOff>
+      <xdr:rowOff>1140</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>424961</xdr:colOff>
+      <xdr:colOff>372667</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>92800</xdr:rowOff>
+      <xdr:rowOff>25565</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3473,8 +4498,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5006729" y="2852606"/>
-          <a:ext cx="742463" cy="210040"/>
+          <a:off x="4962193" y="2802611"/>
+          <a:ext cx="744474" cy="211189"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3885,17 +4910,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="G13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="6" max="6" width="11.08984375" customWidth="1"/>
     <col min="7" max="7" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3909,7 +4934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3932,7 +4957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3951,9 +4976,11 @@
       <c r="F3" s="3">
         <v>0.94279999999999997</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="3">
+        <v>0.96909999999999996</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3972,9 +4999,11 @@
       <c r="F4">
         <v>0.94820000000000004</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="3">
+        <v>0.97140000000000004</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>5</v>
       </c>
@@ -3993,9 +5022,11 @@
       <c r="F5">
         <v>0.95269999999999999</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="3">
+        <v>0.96909999999999996</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>10</v>
       </c>
@@ -4014,9 +5045,11 @@
       <c r="F6" s="2">
         <v>0.96</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="3">
+        <v>0.96730000000000005</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>30</v>
       </c>
@@ -4035,8 +5068,11 @@
       <c r="F7" s="3">
         <v>0.96460000000000001</v>
       </c>
+      <c r="G7" s="3">
+        <v>0.95950000000000002</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>80</v>
       </c>
@@ -4055,36 +5091,39 @@
       <c r="F8" s="3">
         <v>0.9667</v>
       </c>
+      <c r="G8" s="3">
+        <v>0.94689999999999996</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>110</v>
       </c>
       <c r="B9" s="1">
         <v>0.98260000000000003</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="3">
         <v>0.96679999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>150</v>
       </c>
       <c r="B10" s="4">
         <v>0.96819999999999995</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="3">
         <v>0.96519999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -4092,7 +5131,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -4101,7 +5140,9 @@
       <c r="G15" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add rbf related material in final report
</commit_message>
<xml_diff>
--- a/docs/plots.xlsx
+++ b/docs/plots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="0" windowWidth="18070" windowHeight="7540"/>
+    <workbookView xWindow="4520" yWindow="0" windowWidth="18070" windowHeight="7540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4910,8 +4910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Final work and code cleanup
</commit_message>
<xml_diff>
--- a/docs/plots.xlsx
+++ b/docs/plots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7910" yWindow="0" windowWidth="18070" windowHeight="7540"/>
+    <workbookView xWindow="9040" yWindow="0" windowWidth="18070" windowHeight="7540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3005,9 +3005,6 @@
                 <c:pt idx="6">
                   <c:v>0.98260000000000003</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.98399999999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3429,9 +3426,6 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.98260000000000003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.98399999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8513,8 +8507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8589,7 +8583,7 @@
       <c r="G3" s="3">
         <v>0.96909999999999996</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="2">
         <f>1924/2007</f>
         <v>0.95864474339810668</v>
       </c>
@@ -8741,9 +8735,7 @@
       <c r="A10">
         <v>150</v>
       </c>
-      <c r="B10" s="4">
-        <v>0.98399999999999999</v>
-      </c>
+      <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>

</xml_diff>